<commit_message>
Updating code to pilot locations
</commit_message>
<xml_diff>
--- a/collectionList.xlsx
+++ b/collectionList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houstobn\Documents\GitHub\staticPages-webArchives\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WebArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,71 +14,83 @@
   <sheets>
     <sheet name="collectionList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
-  <si>
-    <t>Records</t>
-  </si>
-  <si>
-    <t>ead</t>
-  </si>
-  <si>
-    <t>Collection</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>PRIVATE</t>
-  </si>
-  <si>
-    <t>FORMAT</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>EXTENT</t>
-  </si>
-  <si>
-    <t>UNITS</t>
-  </si>
-  <si>
-    <t>ABSTRACT</t>
-  </si>
-  <si>
-    <t>WebArchiveSeries</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>EAD</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unittitle</t>
+  </si>
+  <si>
+    <t>Scope and Content Note</t>
+  </si>
+  <si>
+    <t>Web Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Collection </t>
   </si>
   <si>
     <t>URL</t>
   </si>
   <si>
-    <t>uwmac0001</t>
-  </si>
-  <si>
-    <t>UWM. College of Letters and Science. Office of the Dean</t>
-  </si>
-  <si>
-    <t>uwmac0030</t>
-  </si>
-  <si>
-    <t>UWM. Department of Dance.</t>
-  </si>
-  <si>
-    <t>uwmac0081</t>
-  </si>
-  <si>
-    <t>UWM. Peck School of the Arts. Office of the Dean.</t>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>uwmac0068</t>
+  </si>
+  <si>
+    <t>UWM. Urban Studies Programs</t>
+  </si>
+  <si>
+    <t>Urban Studies Website</t>
+  </si>
+  <si>
+    <t>http://uwm.edu/urban-studies</t>
+  </si>
+  <si>
+    <t>e.polis</t>
+  </si>
+  <si>
+    <t>http://uwm.edu/urban-studies/research/e-polis</t>
+  </si>
+  <si>
+    <t>50th Anniversary Celebration</t>
+  </si>
+  <si>
+    <t>http://uwm.edu/urban-studies/research/usp-50th-anniversary/</t>
+  </si>
+  <si>
+    <t>Page created in 2013 to celebrate the 50th year of Urban Studies Programs at UWM.</t>
+  </si>
+  <si>
+    <t>Home Page of the Urban Studies Programs.</t>
+  </si>
+  <si>
+    <t>Issues pages for e.polis, the Graduate Student Journal of Urban Studies Programs.</t>
   </si>
 </sst>
 </file>
@@ -572,9 +584,8 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
@@ -636,26 +647,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L174" totalsRowShown="0">
-  <autoFilter ref="A1:L174"/>
-  <sortState ref="A2:I855">
-    <sortCondition ref="A1:A855"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L154" totalsRowShown="0">
+  <autoFilter ref="A1:L154"/>
+  <sortState ref="A2:L6">
+    <sortCondition ref="A1:A170"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="PRIVATE"/>
-    <tableColumn id="3" name="FORMAT"/>
-    <tableColumn id="4" name="TITLE"/>
-    <tableColumn id="5" name="TYPE"/>
-    <tableColumn id="6" name="DATE"/>
-    <tableColumn id="7" name="EXTENT"/>
-    <tableColumn id="8" name="UNITS"/>
-    <tableColumn id="9" name="ABSTRACT"/>
-    <tableColumn id="10" name="WebArchiveSeries"/>
-    <tableColumn id="12" name="Collection"/>
+    <tableColumn id="1" name="EAD"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Unit"/>
+    <tableColumn id="5" name="Type"/>
+    <tableColumn id="6" name="Level"/>
+    <tableColumn id="7" name="Unittitle"/>
+    <tableColumn id="8" name="Series"/>
+    <tableColumn id="9" name="Scope and Content Note"/>
+    <tableColumn id="10" name="Web Series"/>
+    <tableColumn id="12" name="Web Collection "/>
     <tableColumn id="11" name="URL"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -980,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L170"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD174"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +1005,7 @@
     <col min="4" max="4" width="108.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
@@ -1007,131 +1018,144 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3368</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
+      <c r="H3">
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>3368</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
+      <c r="H4">
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L22" s="2"/>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F57" s="1"/>
-    </row>
-    <row r="170" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L170" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>3368</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>